<commit_message>
26-Apr-2024: Codes were modified to support one group of questions in the question bank, e.g. 01A, 02A, ... 01H, 02H, ...
</commit_message>
<xml_diff>
--- a/output/marksheet-01.xlsx
+++ b/output/marksheet-01.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,11 +444,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>M01A</t>
+          <t>02A</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -457,11 +457,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>M03A</t>
+          <t>03A</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -470,11 +470,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>M06A</t>
+          <t>04A</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -483,11 +483,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>M08A</t>
+          <t>05A</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -496,7 +496,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>O09A</t>
+          <t>06A</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -509,11 +509,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>M04B</t>
+          <t>02B</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -522,11 +522,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>M05B</t>
+          <t>03B</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -535,11 +535,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>M08B</t>
+          <t>04B</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -548,7 +548,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>O04B</t>
+          <t>05B</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -561,11 +561,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>O05B</t>
+          <t>10B</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -574,11 +574,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>M07C</t>
+          <t>04C</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -587,11 +587,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>M10C</t>
+          <t>05C</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -600,11 +600,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>O07C</t>
+          <t>06C</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -613,7 +613,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>O08C</t>
+          <t>09C</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -626,11 +626,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>O10C</t>
+          <t>10C</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -639,11 +639,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>N01D</t>
+          <t>04D</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -652,11 +652,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>N08D</t>
+          <t>05D</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -665,11 +665,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>N09D</t>
+          <t>06D</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -678,11 +678,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>O04D</t>
+          <t>08D</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -691,7 +691,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>O06D</t>
+          <t>10D</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -704,11 +704,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>M01E</t>
+          <t>04E</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -717,11 +717,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>M09E</t>
+          <t>05E</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
@@ -730,11 +730,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>O10E</t>
+          <t>07E</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -743,11 +743,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>N01F</t>
+          <t>02F</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
@@ -756,11 +756,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>N10F</t>
+          <t>06F</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
@@ -769,7 +769,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>O01F</t>
+          <t>09F</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -782,11 +782,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>M10G</t>
+          <t>04G</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -795,11 +795,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>O03G</t>
+          <t>06G</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
@@ -808,11 +808,63 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>O05G</t>
+          <t>09G</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>02H</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>05H</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>07H</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>08H</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>